<commit_message>
update readme and lib gen
</commit_message>
<xml_diff>
--- a/3_annotation_manual/HE/2_combine_annotation/all_lab_annotations.xlsx
+++ b/3_annotation_manual/HE/2_combine_annotation/all_lab_annotations.xlsx
@@ -98,7 +98,7 @@
     <t xml:space="preserve">lab_id</t>
   </si>
   <si>
-    <t xml:space="preserve">peak_evidence_rt_grouped_manual_fixed_afekta.xlsx</t>
+    <t xml:space="preserve">fixed_annotation_afekta.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">CP396003|CP395863|CP636221|CP636265</t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">359.090344308663|359.090344308663|350.039258190606|350.039258190606</t>
   </si>
   <si>
-    <t xml:space="preserve">afekta</t>
+    <t xml:space="preserve">_afekta</t>
   </si>
   <si>
     <t xml:space="preserve">CP397041|CP395017|CP025418|CP022171</t>
@@ -6260,7 +6260,7 @@
     <t xml:space="preserve">1474.51981997084|1467.91314813572</t>
   </si>
   <si>
-    <t xml:space="preserve">peak_evidence_rt_grouped_manual_fixed_cembio.xlsx</t>
+    <t xml:space="preserve">fixed_annotation_cembio.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">CP241236|CP492166|CP012382|CP012464</t>
@@ -6269,7 +6269,7 @@
     <t xml:space="preserve">279.592328279252|0|288.898405676557|396.144434223886</t>
   </si>
   <si>
-    <t xml:space="preserve">cembio</t>
+    <t xml:space="preserve">_cembio</t>
   </si>
   <si>
     <t xml:space="preserve">CP262606|CP032129|CP031474</t>
@@ -7880,7 +7880,7 @@
     <t xml:space="preserve">524.904720354607|523.678229436494|523.678229436494</t>
   </si>
   <si>
-    <t xml:space="preserve">peak_evidence_rt_grouped_manual_fixed_hmgu.xlsx</t>
+    <t xml:space="preserve">fixed_annotation_hmgu.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">CP095176|CP013214</t>
@@ -7889,7 +7889,7 @@
     <t xml:space="preserve">252.642427511135|330.922918840406</t>
   </si>
   <si>
-    <t xml:space="preserve">hmgu</t>
+    <t xml:space="preserve">_hmgu</t>
   </si>
   <si>
     <t xml:space="preserve">CP157808|CP058544|CP058538</t>
@@ -9296,13 +9296,13 @@
     <t xml:space="preserve">759.353523801824|759.353523801824</t>
   </si>
   <si>
-    <t xml:space="preserve">peak_evidence_rt_grouped_manual_fixed_icl.xlsx</t>
+    <t xml:space="preserve">fixed_annotation_icl.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">CP018232|CP018250</t>
   </si>
   <si>
-    <t xml:space="preserve">icl</t>
+    <t xml:space="preserve">_icl</t>
   </si>
   <si>
     <t xml:space="preserve">CP444026|CP721301|CP018399</t>

</xml_diff>